<commit_message>
Add experiments 20-23; Add adversarial attack test
</commit_message>
<xml_diff>
--- a/Stein Gradients/Experiments/Results.xlsx
+++ b/Stein Gradients/Experiments/Results.xlsx
@@ -2217,52 +2217,52 @@
         <v>5</v>
       </c>
       <c r="M20">
-        <v>0.285</v>
+        <v>0.03</v>
       </c>
       <c r="N20">
-        <v>0.295</v>
+        <v>0.114</v>
       </c>
       <c r="O20">
-        <v>0.209</v>
+        <v>0.078</v>
       </c>
       <c r="P20">
-        <v>0.189</v>
+        <v>0.067</v>
       </c>
       <c r="Q20">
-        <v>0.919</v>
+        <v>0.99</v>
       </c>
       <c r="R20">
-        <v>0.913</v>
+        <v>0.972</v>
       </c>
       <c r="S20">
-        <v>0.951</v>
+        <v>0.981</v>
       </c>
       <c r="T20">
-        <v>0.949</v>
+        <v>0.981</v>
       </c>
       <c r="U20">
-        <v>0.255</v>
+        <v>0.026</v>
       </c>
       <c r="V20">
-        <v>0.257</v>
+        <v>0.091</v>
       </c>
       <c r="W20">
-        <v>0.209</v>
+        <v>0.078</v>
       </c>
       <c r="X20">
-        <v>0.189</v>
+        <v>0.063</v>
       </c>
       <c r="Y20">
-        <v>0.926</v>
+        <v>0.991</v>
       </c>
       <c r="Z20">
-        <v>0.925</v>
+        <v>0.976</v>
       </c>
       <c r="AA20">
-        <v>0.951</v>
+        <v>0.981</v>
       </c>
       <c r="AB20">
-        <v>0.951</v>
+        <v>0.982</v>
       </c>
       <c r="AC20" t="s">
         <v>26</v>
@@ -2389,52 +2389,52 @@
         <v>5</v>
       </c>
       <c r="M22">
-        <v>0.462</v>
+        <v>0.034</v>
       </c>
       <c r="N22">
-        <v>0.458</v>
+        <v>0.108</v>
       </c>
       <c r="O22">
-        <v>10000000000</v>
+        <v>0.075</v>
       </c>
       <c r="P22">
-        <v>10000000000</v>
+        <v>0.064</v>
       </c>
       <c r="Q22">
-        <v>0.868</v>
+        <v>0.989</v>
       </c>
       <c r="R22">
-        <v>0.867</v>
+        <v>0.972</v>
       </c>
       <c r="S22">
-        <v>0</v>
+        <v>0.982</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="U22">
-        <v>0.398</v>
+        <v>0.024</v>
       </c>
       <c r="V22">
-        <v>0.375</v>
+        <v>0.091</v>
       </c>
       <c r="W22">
-        <v>10000000000</v>
+        <v>0.075</v>
       </c>
       <c r="X22">
-        <v>10000000000</v>
+        <v>0.06</v>
       </c>
       <c r="Y22">
-        <v>0.888</v>
+        <v>0.992</v>
       </c>
       <c r="Z22">
-        <v>0.892</v>
+        <v>0.975</v>
       </c>
       <c r="AA22">
-        <v>0</v>
+        <v>0.982</v>
       </c>
       <c r="AB22">
-        <v>0</v>
+        <v>0.982</v>
       </c>
       <c r="AC22" t="s">
         <v>26</v>
@@ -2478,13 +2478,13 @@
         <v>0.002</v>
       </c>
       <c r="N23">
-        <v>0.091</v>
+        <v>0.093</v>
       </c>
       <c r="O23">
-        <v>10000000000</v>
+        <v>0.093</v>
       </c>
       <c r="P23">
-        <v>10000000000</v>
+        <v>0.093</v>
       </c>
       <c r="Q23">
         <v>1</v>
@@ -2493,10 +2493,10 @@
         <v>0.98</v>
       </c>
       <c r="S23">
-        <v>0</v>
+        <v>0.981</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="U23">
         <v>0.002</v>
@@ -2505,10 +2505,10 @@
         <v>0.08500000000000001</v>
       </c>
       <c r="W23">
-        <v>10000000000</v>
+        <v>0.091</v>
       </c>
       <c r="X23">
-        <v>10000000000</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="Y23">
         <v>1</v>
@@ -2517,10 +2517,10 @@
         <v>0.981</v>
       </c>
       <c r="AA23">
-        <v>0</v>
+        <v>0.981</v>
       </c>
       <c r="AB23">
-        <v>0</v>
+        <v>0.981</v>
       </c>
       <c r="AC23" t="s">
         <v>26</v>
@@ -3358,22 +3358,22 @@
         <v>5</v>
       </c>
       <c r="G20">
-        <v>0.913</v>
+        <v>0.972</v>
       </c>
       <c r="H20">
-        <v>0.925</v>
+        <v>0.976</v>
       </c>
       <c r="I20">
-        <v>0.951</v>
+        <v>0.981</v>
       </c>
       <c r="J20">
-        <v>0.951</v>
+        <v>0.981</v>
       </c>
       <c r="K20">
-        <v>0.949</v>
+        <v>0.981</v>
       </c>
       <c r="L20">
-        <v>0.951</v>
+        <v>0.982</v>
       </c>
       <c r="M20" t="s">
         <v>26</v>
@@ -3440,22 +3440,22 @@
         <v>5</v>
       </c>
       <c r="G22">
-        <v>0.867</v>
+        <v>0.972</v>
       </c>
       <c r="H22">
-        <v>0.892</v>
+        <v>0.975</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>0.982</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>0.982</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>0.982</v>
       </c>
       <c r="M22" t="s">
         <v>26</v>
@@ -3487,16 +3487,16 @@
         <v>0.981</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>0.981</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>0.981</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>0.981</v>
       </c>
       <c r="M23" t="s">
         <v>26</v>

</xml_diff>